<commit_message>
Add evaluate_all command for numeric_model
</commit_message>
<xml_diff>
--- a/app/models/tables/numeric_model/test.xlsx
+++ b/app/models/tables/numeric_model/test.xlsx
@@ -477,25 +477,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7180811808118082</v>
+        <v>0.7281672816728167</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4463667820069204</v>
+        <v>0.4575278265963679</v>
       </c>
       <c r="D2" t="n">
-        <v>0.80625</v>
+        <v>0.8135416666666667</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5746102449888641</v>
+        <v>0.5856767904011998</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4268638582949109</v>
+        <v>0.4434542885967195</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3887963914178092</v>
+        <v>0.4061507830270435</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7485356280193236</v>
+        <v>0.7576565016103061</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Add figures and normalize
</commit_message>
<xml_diff>
--- a/app/models/tables/numeric_model/test.xlsx
+++ b/app/models/tables/numeric_model/test.xlsx
@@ -557,29 +557,29 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>xgb</t>
+          <t>xgbclassifier</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7284132841328413</v>
+        <v>0.7345633456334564</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4568345323741007</v>
+        <v>0.4632489190858555</v>
       </c>
       <c r="D5" t="n">
-        <v>0.79375</v>
+        <v>0.78125</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5799086757990868</v>
+        <v>0.5816207832493214</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4334167632146244</v>
+        <v>0.4349914851328425</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4000529393363332</v>
+        <v>0.4052823296595123</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7509812801932367</v>
+        <v>0.7506894122383253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>